<commit_message>
Session 04 files updated in session
</commit_message>
<xml_diff>
--- a/hands_on_exercises/session04/Patient Story - Mapping.xlsx
+++ b/hands_on_exercises/session04/Patient Story - Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\FBT2K24\hands_on_exercises\session04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005BECA2-F6E4-4916-8DCB-F6009D293ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D579DB9F-7758-4483-BB14-F1703A85BED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstPage" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
   <si>
     <t>Sl</t>
   </si>
@@ -169,6 +169,114 @@
   </si>
   <si>
     <t>PHR</t>
+  </si>
+  <si>
+    <t>Ravindranath</t>
+  </si>
+  <si>
+    <t>Phlebotomist Deepak</t>
+  </si>
+  <si>
+    <t>patient’s left arm</t>
+  </si>
+  <si>
+    <t>R587439-002</t>
+  </si>
+  <si>
+    <t>Lavender Top</t>
+  </si>
+  <si>
+    <t>3 ml</t>
+  </si>
+  <si>
+    <t>R587439-003</t>
+  </si>
+  <si>
+    <t>R587439-004</t>
+  </si>
+  <si>
+    <t>Green Top</t>
+  </si>
+  <si>
+    <t>2 ml</t>
+  </si>
+  <si>
+    <t>NMR tube carrier</t>
+  </si>
+  <si>
+    <t>CBC</t>
+  </si>
+  <si>
+    <t>Troponin I</t>
+  </si>
+  <si>
+    <t>Troponin T</t>
+  </si>
+  <si>
+    <t>whole blood</t>
+  </si>
+  <si>
+    <t>Specimen.type</t>
+  </si>
+  <si>
+    <t>Code: BLD
+Dispplay: Whole blood
+Code System URL: http://terminology.hl7.org/CodeSystem/v2-0487
+Value Set URL:	http://terminology.hl7.org/ValueSet/v2-0487</t>
+  </si>
+  <si>
+    <t>Specimen.subject</t>
+  </si>
+  <si>
+    <t>Specimen.subject.reference = Resource ID
+Specimen.subject.type = Patient</t>
+  </si>
+  <si>
+    <t>Specimen.collection.collector</t>
+  </si>
+  <si>
+    <t>Specimen.collection.collector.reference = ResourceID
+Specimen.collection.collector.type = Practitioner</t>
+  </si>
+  <si>
+    <t>Specimen.collection.bodySite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specimen.collection.bodySite.coding.system =  
+http://snomed.info/sct
+Specimen.collection.bodySite.coding.code = 
+368208006
+Specimen.collection.bodySite.coding.display = 
+Left arm
+</t>
+  </si>
+  <si>
+    <t>Specimen.request</t>
+  </si>
+  <si>
+    <t>Not mapped</t>
+  </si>
+  <si>
+    <t>Expected to be part of ServiceRequest</t>
+  </si>
+  <si>
+    <t>Should link to the ServiceRequest</t>
+  </si>
+  <si>
+    <t>Specimen.accessionIdentifier.value</t>
+  </si>
+  <si>
+    <t>Specimen.container.description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specimen.collection.quantity.value = 3
+Specimen.collection.quantity.unit = ml
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specimen.collection.quantity.value = 2
+Specimen.collection.quantity.unit = ml
+</t>
   </si>
 </sst>
 </file>
@@ -176,7 +284,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd/mmmm/yy"/>
+    <numFmt numFmtId="164" formatCode="dd/mmmm/yy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -195,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +313,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -250,7 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -258,6 +372,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,9 +666,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +972,7 @@
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,19 +1744,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520DA2D5-B615-4585-B164-F550A97A92FA}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1648,125 +1774,221 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="B5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="9">
+        <v>87349301</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="12"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
+      <c r="B13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="9">
+        <v>87349302</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Session 04 files updated for all three groups
</commit_message>
<xml_diff>
--- a/hands_on_exercises/session04/Patient Story - Mapping.xlsx
+++ b/hands_on_exercises/session04/Patient Story - Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\FBT2K24\hands_on_exercises\session04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D579DB9F-7758-4483-BB14-F1703A85BED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DA6ED9-3550-4F00-A393-1B6A5D701D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstPage" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="119">
   <si>
     <t>Sl</t>
   </si>
@@ -277,6 +277,138 @@
     <t xml:space="preserve">Specimen.collection.quantity.value = 2
 Specimen.collection.quantity.unit = ml
 </t>
+  </si>
+  <si>
+    <t>ECG → Cath Lab (Order ID: R587439-001)</t>
+  </si>
+  <si>
+    <t>ServiceRequest.identifer.value</t>
+  </si>
+  <si>
+    <t>R587439</t>
+  </si>
+  <si>
+    <t>ServiceRequest.requisition.value</t>
+  </si>
+  <si>
+    <t>R587439-001</t>
+  </si>
+  <si>
+    <t>ServiceRequest.status</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>ServiceRequest.intent</t>
+  </si>
+  <si>
+    <t>original-order</t>
+  </si>
+  <si>
+    <t>ServiceRequest.priority</t>
+  </si>
+  <si>
+    <t>urgent</t>
+  </si>
+  <si>
+    <t>ServiceRequest.code.coding.system</t>
+  </si>
+  <si>
+    <t>http://snomed.info/sct</t>
+  </si>
+  <si>
+    <t>ServiceRequest.code.coding.code</t>
+  </si>
+  <si>
+    <t>ServiceRequest.code.coding.display</t>
+  </si>
+  <si>
+    <t>Electrocardiographic procedure</t>
+  </si>
+  <si>
+    <t>ServiceRequest.quantityQuantity.value</t>
+  </si>
+  <si>
+    <t>ServiceRequest.reruester</t>
+  </si>
+  <si>
+    <t>Use PractitionerRole Resource Instance - Dr. Sid</t>
+  </si>
+  <si>
+    <t>ServiceRequest.subject</t>
+  </si>
+  <si>
+    <t>Use the Patient Resource Instance</t>
+  </si>
+  <si>
+    <t>Rohan</t>
+  </si>
+  <si>
+    <t>Practitioner.name.given</t>
+  </si>
+  <si>
+    <t>Receptionist (occupation)</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.display</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.code</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.system</t>
+  </si>
+  <si>
+    <t>Practitioner/id_of_rohan</t>
+  </si>
+  <si>
+    <t>PractitionerRole.practitioner</t>
+  </si>
+  <si>
+    <t>Organization/id_of_getwellsoonhospital</t>
+  </si>
+  <si>
+    <t>PractitionerRole.organization</t>
+  </si>
+  <si>
+    <t>HealthcareService.name</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/service-type</t>
+  </si>
+  <si>
+    <t>HealthcareService.type.coding.code.system</t>
+  </si>
+  <si>
+    <t>HealthcareService.type.coding.code.code</t>
+  </si>
+  <si>
+    <t>Diag. Radiology /Xray /CT /Fluoroscopy</t>
+  </si>
+  <si>
+    <t>HealthcareService.type.coding.code.display</t>
+  </si>
+  <si>
+    <t>Akanksha</t>
+  </si>
+  <si>
+    <t>Nurse</t>
+  </si>
+  <si>
+    <t>nurse</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/practitioner-role</t>
+  </si>
+  <si>
+    <t>Practitioner/id_of_Akanksha</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>Encounter.status</t>
   </si>
 </sst>
 </file>
@@ -286,7 +418,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmmm/yy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,8 +434,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,8 +462,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -346,11 +492,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -384,8 +544,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -666,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
@@ -1430,19 +1612,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B24B16F9-A33C-4BE0-91B5-6721B5195B1F}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1464,89 +1649,135 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="9">
+        <v>29303009</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -1581,6 +1812,9 @@
       <c r="D16" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{DA88DB53-20C4-4F1F-808B-1D0A8A1EDB46}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1744,9 +1978,12 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520DA2D5-B615-4585-B164-F550A97A92FA}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
@@ -1970,7 +2207,7 @@
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1997,158 +2234,251 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7725F43-764F-4712-8E7E-E2923B30D7F1}">
-  <dimension ref="A1:D16"/>
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="44.140625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="B4" s="17">
+        <v>159561009</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="B5" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="16">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="16">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="B10" s="17">
+        <v>209</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>111</v>
+      </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="16">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="B12" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="16">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="B14" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="16">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <v>16</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>17</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{1070002D-7EC0-4461-90E9-37BE08CDE708}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{6D416DC3-4AA2-41B2-B82F-B6C977686DC7}"/>
+    <hyperlink ref="B15" r:id="rId3" xr:uid="{0E5446BC-CB41-417A-88B7-C439B83DC21A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>